<commit_message>
Before python script writing
</commit_message>
<xml_diff>
--- a/sound_files/originals/AUD-20231221-WA0007_5th.m4aBall_Bounces.xlsx
+++ b/sound_files/originals/AUD-20231221-WA0007_5th.m4aBall_Bounces.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,22 +470,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>23665</v>
+        <v>161948</v>
       </c>
       <c r="C2" t="n">
-        <v>64606</v>
+        <v>244979</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.007916307322576475</v>
+        <v>0.0003129578401736774</v>
       </c>
       <c r="F2" t="n">
-        <v>324</v>
+        <v>25</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8529375</v>
+        <v>1.7298125</v>
       </c>
     </row>
     <row r="3">
@@ -493,22 +493,22 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>161948</v>
+        <v>382802</v>
       </c>
       <c r="C3" t="n">
-        <v>244979</v>
+        <v>463035</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01008204190161307</v>
+        <v>0.0003324682364840729</v>
       </c>
       <c r="F3" t="n">
-        <v>837</v>
+        <v>26</v>
       </c>
       <c r="G3" t="n">
-        <v>1.7298125</v>
+        <v>1.671520833333333</v>
       </c>
     </row>
     <row r="4">
@@ -516,22 +516,22 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>245283</v>
+        <v>623421</v>
       </c>
       <c r="C4" t="n">
-        <v>247607</v>
+        <v>696421</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01448849598780044</v>
+        <v>0.0003447825584320573</v>
       </c>
       <c r="F4" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04841666666666666</v>
+        <v>1.520833333333333</v>
       </c>
     </row>
     <row r="5">
@@ -539,22 +539,22 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>255413</v>
+        <v>860835</v>
       </c>
       <c r="C5" t="n">
-        <v>261273</v>
+        <v>941178</v>
       </c>
       <c r="D5" t="n">
         <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01260439942201318</v>
+        <v>0.0003158486840906858</v>
       </c>
       <c r="F5" t="n">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1220833333333333</v>
+        <v>1.6738125</v>
       </c>
     </row>
     <row r="6">
@@ -562,22 +562,22 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>382802</v>
+        <v>1089941</v>
       </c>
       <c r="C6" t="n">
-        <v>463035</v>
+        <v>1175641</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>0.01012468993058937</v>
+        <v>0.0003151987174443318</v>
       </c>
       <c r="F6" t="n">
-        <v>812</v>
+        <v>27</v>
       </c>
       <c r="G6" t="n">
-        <v>1.671520833333333</v>
+        <v>1.785416666666667</v>
       </c>
     </row>
     <row r="7">
@@ -585,22 +585,22 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>567537</v>
+        <v>1340788</v>
       </c>
       <c r="C7" t="n">
-        <v>569614</v>
+        <v>1418583</v>
       </c>
       <c r="D7" t="n">
         <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1077873231963005</v>
+        <v>0.0003356194075263681</v>
       </c>
       <c r="F7" t="n">
-        <v>223</v>
+        <v>26</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04327083333333333</v>
+        <v>1.620729166666667</v>
       </c>
     </row>
     <row r="8">
@@ -608,22 +608,22 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>623421</v>
+        <v>1601723</v>
       </c>
       <c r="C8" t="n">
-        <v>696421</v>
+        <v>1677283</v>
       </c>
       <c r="D8" t="n">
         <v>6</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01234877706892392</v>
+        <v>0.0003266193185950776</v>
       </c>
       <c r="F8" t="n">
-        <v>901</v>
+        <v>24</v>
       </c>
       <c r="G8" t="n">
-        <v>1.520833333333333</v>
+        <v>1.574166666666667</v>
       </c>
     </row>
     <row r="9">
@@ -631,22 +631,22 @@
         <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>797181</v>
+        <v>1843637</v>
       </c>
       <c r="C9" t="n">
-        <v>799202</v>
+        <v>1932037</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
       </c>
       <c r="E9" t="n">
-        <v>0.08869420773206119</v>
+        <v>0.0003132989066591715</v>
       </c>
       <c r="F9" t="n">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04210416666666666</v>
+        <v>1.841666666666667</v>
       </c>
     </row>
     <row r="10">
@@ -654,22 +654,22 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>860835</v>
+        <v>2094213</v>
       </c>
       <c r="C10" t="n">
-        <v>941178</v>
+        <v>2179909</v>
       </c>
       <c r="D10" t="n">
         <v>8</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0134398745774729</v>
+        <v>0.000335796404248806</v>
       </c>
       <c r="F10" t="n">
-        <v>1079</v>
+        <v>28</v>
       </c>
       <c r="G10" t="n">
-        <v>1.6738125</v>
+        <v>1.785333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -677,22 +677,22 @@
         <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>1089941</v>
+        <v>2369898</v>
       </c>
       <c r="C11" t="n">
-        <v>1175641</v>
+        <v>2464503</v>
       </c>
       <c r="D11" t="n">
         <v>9</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01429574742078653</v>
+        <v>0.0003305113983761532</v>
       </c>
       <c r="F11" t="n">
-        <v>1225</v>
+        <v>31</v>
       </c>
       <c r="G11" t="n">
-        <v>1.785416666666667</v>
+        <v>1.9709375</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>1340788</v>
+        <v>2639490</v>
       </c>
       <c r="C12" t="n">
-        <v>1418583</v>
+        <v>2716124</v>
       </c>
       <c r="D12" t="n">
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01129946558463752</v>
+        <v>0.0003465508901238823</v>
       </c>
       <c r="F12" t="n">
-        <v>879</v>
+        <v>26</v>
       </c>
       <c r="G12" t="n">
-        <v>1.620729166666667</v>
+        <v>1.596541666666667</v>
       </c>
     </row>
     <row r="13">
@@ -723,22 +723,22 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>1514523</v>
+        <v>2894082</v>
       </c>
       <c r="C13" t="n">
-        <v>1516783</v>
+        <v>2965592</v>
       </c>
       <c r="D13" t="n">
         <v>11</v>
       </c>
       <c r="E13" t="n">
-        <v>0.08250934734177762</v>
+        <v>0.0003715089033179772</v>
       </c>
       <c r="F13" t="n">
-        <v>186</v>
+        <v>26</v>
       </c>
       <c r="G13" t="n">
-        <v>0.04708333333333333</v>
+        <v>1.489791666666667</v>
       </c>
     </row>
     <row r="14">
@@ -746,389 +746,21 @@
         <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>1516923</v>
+        <v>3151039</v>
       </c>
       <c r="C14" t="n">
-        <v>1519108</v>
+        <v>3228596</v>
       </c>
       <c r="D14" t="n">
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>0.05727844139699715</v>
+        <v>0.0003470899048190195</v>
       </c>
       <c r="F14" t="n">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="G14" t="n">
-        <v>0.04552083333333334</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1601723</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1677283</v>
-      </c>
-      <c r="D15" t="n">
-        <v>13</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.0244254080563262</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1845</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1.574166666666667</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1677407</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1681169</v>
-      </c>
-      <c r="D16" t="n">
-        <v>14</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.01410403377853962</v>
-      </c>
-      <c r="F16" t="n">
-        <v>53</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.078375</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1798119</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1802294</v>
-      </c>
-      <c r="D17" t="n">
-        <v>15</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.1336508175888994</v>
-      </c>
-      <c r="F17" t="n">
-        <v>557</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.08697916666666666</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1843637</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1932037</v>
-      </c>
-      <c r="D18" t="n">
-        <v>16</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.02503386338157495</v>
-      </c>
-      <c r="F18" t="n">
-        <v>2212</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1.841666666666667</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B19" t="n">
-        <v>2033374</v>
-      </c>
-      <c r="C19" t="n">
-        <v>2037618</v>
-      </c>
-      <c r="D19" t="n">
-        <v>17</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.05559690406164207</v>
-      </c>
-      <c r="F19" t="n">
-        <v>235</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.08841666666666667</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B20" t="n">
-        <v>2094213</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2179909</v>
-      </c>
-      <c r="D20" t="n">
-        <v>18</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.02496712629397323</v>
-      </c>
-      <c r="F20" t="n">
-        <v>2139</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1.785333333333333</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B21" t="n">
-        <v>2180071</v>
-      </c>
-      <c r="C21" t="n">
-        <v>2182760</v>
-      </c>
-      <c r="D21" t="n">
-        <v>19</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.02450194008185587</v>
-      </c>
-      <c r="F21" t="n">
-        <v>65</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.05602083333333333</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B22" t="n">
-        <v>2369898</v>
-      </c>
-      <c r="C22" t="n">
-        <v>2464503</v>
-      </c>
-      <c r="D22" t="n">
-        <v>20</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.02450805187603399</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2318</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1.9709375</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B23" t="n">
-        <v>2639490</v>
-      </c>
-      <c r="C23" t="n">
-        <v>2716124</v>
-      </c>
-      <c r="D23" t="n">
-        <v>21</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.02479069573251338</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1899</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1.596541666666667</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B24" t="n">
-        <v>2828023</v>
-      </c>
-      <c r="C24" t="n">
-        <v>2830207</v>
-      </c>
-      <c r="D24" t="n">
-        <v>22</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.05157516905584442</v>
-      </c>
-      <c r="F24" t="n">
-        <v>112</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.0455</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B25" t="n">
-        <v>2837318</v>
-      </c>
-      <c r="C25" t="n">
-        <v>2839484</v>
-      </c>
-      <c r="D25" t="n">
-        <v>23</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.0112224111217103</v>
-      </c>
-      <c r="F25" t="n">
-        <v>24</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.045125</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B26" t="n">
-        <v>2894082</v>
-      </c>
-      <c r="C26" t="n">
-        <v>2965592</v>
-      </c>
-      <c r="D26" t="n">
-        <v>24</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.014572349696263</v>
-      </c>
-      <c r="F26" t="n">
-        <v>1042</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1.489791666666667</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B27" t="n">
-        <v>2976672</v>
-      </c>
-      <c r="C27" t="n">
-        <v>2978675</v>
-      </c>
-      <c r="D27" t="n">
-        <v>25</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.04535896756996644</v>
-      </c>
-      <c r="F27" t="n">
-        <v>90</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.04172916666666666</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B28" t="n">
-        <v>2990363</v>
-      </c>
-      <c r="C28" t="n">
-        <v>2992568</v>
-      </c>
-      <c r="D28" t="n">
-        <v>26</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.01115775768153579</v>
-      </c>
-      <c r="F28" t="n">
-        <v>24</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.0459375</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B29" t="n">
-        <v>3069322</v>
-      </c>
-      <c r="C29" t="n">
-        <v>3074098</v>
-      </c>
-      <c r="D29" t="n">
-        <v>27</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.08149757496994559</v>
-      </c>
-      <c r="F29" t="n">
-        <v>389</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.09950000000000001</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B30" t="n">
-        <v>3151039</v>
-      </c>
-      <c r="C30" t="n">
-        <v>3228596</v>
-      </c>
-      <c r="D30" t="n">
-        <v>28</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.01425335569960458</v>
-      </c>
-      <c r="F30" t="n">
-        <v>1105</v>
-      </c>
-      <c r="G30" t="n">
         <v>1.615770833333333</v>
       </c>
     </row>

</xml_diff>